<commit_message>
Switch to spreadsheet text input in welcome and what is pages
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2DF6D2E-885F-4C46-A8FD-4C20B14ED73E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7A6C6-E98C-4319-B1BD-2DC6F0B684A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="landing" sheetId="1" r:id="rId1"/>
-    <sheet name="setup" sheetId="2" r:id="rId2"/>
-    <sheet name="scenario" sheetId="3" r:id="rId3"/>
-    <sheet name="output" sheetId="4" r:id="rId4"/>
+    <sheet name="welcome" sheetId="1" r:id="rId1"/>
+    <sheet name="what_is" sheetId="5" r:id="rId2"/>
+    <sheet name="setup" sheetId="2" r:id="rId3"/>
+    <sheet name="scenario" sheetId="3" r:id="rId4"/>
+    <sheet name="output" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>reference</t>
   </si>
@@ -187,6 +188,46 @@
   </si>
   <si>
     <t>Want to save these parameters so you can easily use them again later?</t>
+  </si>
+  <si>
+    <t>Welcome to the Devon Air Ambulance Simulation Model</t>
+  </si>
+  <si>
+    <t>Coming Soon!</t>
+  </si>
+  <si>
+    <t>tab_1_name</t>
+  </si>
+  <si>
+    <t>tab_2_name</t>
+  </si>
+  <si>
+    <t>tab_3_name</t>
+  </si>
+  <si>
+    <t>tab_1_content</t>
+  </si>
+  <si>
+    <t>tab_2_content</t>
+  </si>
+  <si>
+    <t>tab_3_content</t>
+  </si>
+  <si>
+    <t>An Introduction to Discrete Event Simulation Modelling</t>
+  </si>
+  <si>
+    <t>This page will introduce you to the fundamental concepts of the computer simulation techniques used in this model.
+No prior knowledge of computer simulation, maths or data science will be required.</t>
+  </si>
+  <si>
+    <t>An Introduction to Simulation Modelling</t>
+  </si>
+  <si>
+    <t>Benefits of Simulation Modelling</t>
+  </si>
+  <si>
+    <t>Limitations of Simulation Modelling</t>
   </si>
 </sst>
 </file>
@@ -354,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -376,15 +417,21 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
@@ -393,6 +440,97 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8933C79-6EBB-4AC4-9B12-31049F780625}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="71.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -616,7 +754,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -647,7 +785,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add placeholders for glossary and info text
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C7A6C6-E98C-4319-B1BD-2DC6F0B684A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC57EDF-5BE4-4C0E-8714-F978FD984042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
-    <sheet name="what_is" sheetId="5" r:id="rId2"/>
-    <sheet name="setup" sheetId="2" r:id="rId3"/>
-    <sheet name="scenario" sheetId="3" r:id="rId4"/>
-    <sheet name="output" sheetId="4" r:id="rId5"/>
+    <sheet name="setup" sheetId="2" r:id="rId2"/>
+    <sheet name="compare_scenarios" sheetId="3" r:id="rId3"/>
+    <sheet name="model" sheetId="4" r:id="rId4"/>
+    <sheet name="what_is" sheetId="5" r:id="rId5"/>
+    <sheet name="info" sheetId="6" r:id="rId6"/>
+    <sheet name="glossary" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,12 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
   <si>
     <t>reference</t>
-  </si>
-  <si>
-    <t>name</t>
   </si>
   <si>
     <t>text</t>
@@ -228,6 +227,58 @@
   </si>
   <si>
     <t>Limitations of Simulation Modelling</t>
+  </si>
+  <si>
+    <t>Glossary of Modelling Terms</t>
+  </si>
+  <si>
+    <t>This page will allow you to look up key terms used throughout this application.</t>
+  </si>
+  <si>
+    <t>Model Information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This page will give an overview of the specifics of how the model works, including how it 
+- generates realistic calls
+- determines what happens to patients at each point in their journey
+- models factors affecting the availability of resources
+and more. Click through the tabs below to read more about the area you are interested in. </t>
+  </si>
+  <si>
+    <t>tab_4_name</t>
+  </si>
+  <si>
+    <t>tab_4_content</t>
+  </si>
+  <si>
+    <t>## How has the data for demand been calculated?
+Coming Soon!
+## Isn't this an underestimate of the true demand?
+Coming Soon!</t>
+  </si>
+  <si>
+    <t>## How are stand-downs calculated?
+Coming Soon!</t>
+  </si>
+  <si>
+    <t>## How are the durations of calls calculated?
+Coming Soon!</t>
+  </si>
+  <si>
+    <t>Summary of Model Logic</t>
+  </si>
+  <si>
+    <t>Demand Data</t>
+  </si>
+  <si>
+    <t>Activity Durations</t>
+  </si>
+  <si>
+    <t>Stand-downs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The diagram below gives a detailed overview of the decision-making process of the model. 
+If you are interested in one particular aspect, try the relevant tab on this page to read more about how decisions are made. </t>
   </si>
 </sst>
 </file>
@@ -410,23 +461,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -440,97 +491,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8933C79-6EBB-4AC4-9B12-31049F780625}">
-  <dimension ref="A1:B9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="71.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -549,199 +509,227 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="132" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
         <v>43</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
         <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
         <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
-        <v>50</v>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -755,24 +743,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C2"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -786,32 +771,242 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8933C79-6EBB-4AC4-9B12-31049F780625}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" activeCellId="1" sqref="A1:C2 E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="71.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EDA8F5-689A-46D5-BBAC-DC7FC0FF134A}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.109375" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="105.6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="66" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6F9923-FCA6-4ECB-A772-03AE65BB7C38}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ensure strict openxlsx format not lost
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr/>
+  <workbookPr dateCompatibility="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC57EDF-5BE4-4C0E-8714-F978FD984042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F189B728-832D-4595-AED8-F2A1E6905CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,10 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
+    <ext xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="77">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="106" uniqueCount="77">
   <si>
     <t>reference</t>
   </si>
@@ -284,7 +287,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -302,8 +305,8 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -335,7 +338,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="LibreOffice">
       <a:dk1>
@@ -443,7 +446,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -491,7 +494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -715,7 +718,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -743,7 +746,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -771,7 +774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8933C79-6EBB-4AC4-9B12-31049F780625}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8933C79-6EBB-4AC4-9B12-31049F780625}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -862,7 +865,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EDA8F5-689A-46D5-BBAC-DC7FC0FF134A}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EDA8F5-689A-46D5-BBAC-DC7FC0FF134A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -969,7 +972,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6F9923-FCA6-4ECB-A772-03AE65BB7C38}">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B6F9923-FCA6-4ECB-A772-03AE65BB7C38}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Add in visualisation of calls per hour
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F189B728-832D-4595-AED8-F2A1E6905CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7452B0F9-044F-45F4-9FC4-AA0EAE93FDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3396" windowWidth="23256" windowHeight="13896" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="106" uniqueCount="77">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="83">
   <si>
     <t>reference</t>
   </si>
@@ -283,16 +283,39 @@
     <t xml:space="preserve">The diagram below gives a detailed overview of the decision-making process of the model. 
 If you are interested in one particular aspect, try the relevant tab on this page to read more about how decisions are made. </t>
   </si>
+  <si>
+    <t>help_jobs_per_hour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This toggle will change the vertical axis to represent the average jobs received per hour rather than the total number of calls received across the full duration of the simulation. This can be better for comparing simulations of different lengths. 
+Lower values indicate fewer calls were received, on average, per hour. Remember that it is possible to receive 0 calls in a given hour some of the time. </t>
+  </si>
+  <si>
+    <t>missed_calls_description</t>
+  </si>
+  <si>
+    <t>These are the 'missed' calls where no DAAT resource was available. This could be due to no resource being on shift, or all resources being tasked to other jobs at the time of the call.</t>
+  </si>
+  <si>
+    <t>This is how much of the available time (where a helicopter is on shift) the helicopter was in use for.</t>
+  </si>
+  <si>
+    <t>helicopter_utilisation_description</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -315,10 +338,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,13 +479,13 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.6640625" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -475,7 +501,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -501,13 +527,13 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="28.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -515,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="38.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -523,7 +549,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -531,7 +557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -539,7 +565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="132" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="127.5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -547,7 +573,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -555,7 +581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -563,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -571,7 +597,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -579,7 +605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -587,7 +613,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -595,7 +621,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -603,7 +629,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -611,7 +637,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -619,7 +645,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -627,7 +653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -635,7 +661,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -643,7 +669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>30</v>
       </c>
@@ -651,7 +677,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -659,7 +685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="51">
       <c r="A20" t="s">
         <v>33</v>
       </c>
@@ -667,7 +693,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -675,7 +701,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -683,7 +709,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -691,7 +717,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -699,7 +725,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -725,9 +751,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -747,20 +773,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="84" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="76.5">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="39" customHeight="1">
+      <c r="A4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -781,13 +835,13 @@
       <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="71.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -803,7 +857,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="51">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -811,7 +865,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -819,7 +873,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -827,7 +881,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -835,7 +889,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -843,7 +897,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -851,7 +905,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -868,17 +922,17 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EDA8F5-689A-46D5-BBAC-DC7FC0FF134A}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="2" width="69.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="69.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -886,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -894,7 +948,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="105.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="102">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -902,7 +956,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -910,7 +964,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -918,7 +972,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -926,7 +980,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -934,7 +988,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="66" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="63.75">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -942,7 +996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="89.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -950,7 +1004,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="38.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -958,7 +1012,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="38.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -979,13 +1033,13 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="83.21875" customWidth="1"/>
+    <col min="2" max="2" width="83.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1001,7 +1055,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Put in some starter text on the welcome page
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7452B0F9-044F-45F4-9FC4-AA0EAE93FDCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{74091915-0956-49E3-AC9F-C74C7A11F819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9810" yWindow="0" windowWidth="17250" windowHeight="9990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="83">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="84">
   <si>
     <t>reference</t>
   </si>
@@ -301,6 +301,16 @@
   </si>
   <si>
     <t>helicopter_utilisation_description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This tool provides an interactive way to explore the operational performance of Devon Air Ambulance. This model helps assess how different factors—such as demand, operating hours and aircraft models—affect patient outcomes and the service as a whole. 
+This tool uses a computer simulation technique called Discrete Event Simulation (DES). A simulated representation of the Devon Air Ambulance service has been built using historical data and service knowledge to replicate the service in a virtual world.
+## How Can the Model be Used?
+The virtual world can run multiple simulations of the same day, month or year, with the timing and nature of calls varying realistically - so you're not just testing against the 'average' day, week or year that the service sees, and can instead stress test a service, testing how it will manage on a 'bad' day too. 
+In addition, by changing the parameters of the simulation, users can assess different "what-if" scenarios—such as adjusting the operating hours or exploring the impact of demand being 10% higher than currently observed.
+The model outputs a range of metrics and graphs, allowing the predicted impact of a change to be interrogated.
+## Getting Started
+Use this interface to run simulations, explore data, and generate insights to support operational planning. </t>
   </si>
 </sst>
 </file>
@@ -475,8 +485,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -501,12 +511,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="357">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>51</v>
+      <c r="B3" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -775,7 +785,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixes to rota text to address #116
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{74091915-0956-49E3-AC9F-C74C7A11F819}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37461788-76EA-4E41-AB24-AB1561AA6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9810" yWindow="0" windowWidth="17250" windowHeight="9990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
@@ -134,12 +134,6 @@
     <t>winter_rota_help</t>
   </si>
   <si>
-    <t>☀️ Summer Rota runs from March to October</t>
-  </si>
-  <si>
-    <t>❄️ Winter Rota runs from November to February</t>
-  </si>
-  <si>
     <t>scenario_comparison_help</t>
   </si>
   <si>
@@ -311,6 +305,12 @@
 The model outputs a range of metrics and graphs, allowing the predicted impact of a change to be interrogated.
 ## Getting Started
 Use this interface to run simulations, explore data, and generate insights to support operational planning. </t>
+  </si>
+  <si>
+    <t>☀️ Summer Rota runs from April to September</t>
+  </si>
+  <si>
+    <t>❄️ Winter Rota runs from October to March</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="357">
@@ -516,7 +516,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -636,7 +636,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -649,10 +649,10 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -676,7 +676,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>31</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -684,63 +684,63 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="51">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -805,26 +805,26 @@
     </row>
     <row r="2" spans="1:2" ht="76.5">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="39" customHeight="1">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -864,7 +864,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="51">
@@ -872,55 +872,55 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -955,7 +955,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="102">
@@ -963,71 +963,71 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="63.75">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="89.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="38.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="38.25">
       <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1062,7 +1062,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add details to 'model details' page
</commit_message>
<xml_diff>
--- a/app/assets/text.xlsx
+++ b/app/assets/text.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DAAT\DAA_DES\app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{37461788-76EA-4E41-AB24-AB1561AA6BEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9F9E334-2827-4652-8657-C6048B2F96BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="welcome" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="84">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="116" uniqueCount="88">
   <si>
     <t>reference</t>
   </si>
@@ -235,33 +235,12 @@
     <t>Model Information</t>
   </si>
   <si>
-    <t xml:space="preserve">This page will give an overview of the specifics of how the model works, including how it 
-- generates realistic calls
-- determines what happens to patients at each point in their journey
-- models factors affecting the availability of resources
-and more. Click through the tabs below to read more about the area you are interested in. </t>
-  </si>
-  <si>
     <t>tab_4_name</t>
   </si>
   <si>
     <t>tab_4_content</t>
   </si>
   <si>
-    <t>## How has the data for demand been calculated?
-Coming Soon!
-## Isn't this an underestimate of the true demand?
-Coming Soon!</t>
-  </si>
-  <si>
-    <t>## How are stand-downs calculated?
-Coming Soon!</t>
-  </si>
-  <si>
-    <t>## How are the durations of calls calculated?
-Coming Soon!</t>
-  </si>
-  <si>
     <t>Summary of Model Logic</t>
   </si>
   <si>
@@ -269,9 +248,6 @@
   </si>
   <si>
     <t>Activity Durations</t>
-  </si>
-  <si>
-    <t>Stand-downs</t>
   </si>
   <si>
     <t xml:space="preserve">The diagram below gives a detailed overview of the decision-making process of the model. 
@@ -311,6 +287,70 @@
   </si>
   <si>
     <t>❄️ Winter Rota runs from October to March</t>
+  </si>
+  <si>
+    <t>Stand-downs and Patient Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This page will give an overview of the specifics of how the model works, including how it 
+- generates realistic calls
+- determines what happens to patients at each point in their journey
+- models factors affecting the availability of resources
+and more. Click through the tabs below to read more about the area you are interested in. </t>
+  </si>
+  <si>
+    <t>tab_5_content</t>
+  </si>
+  <si>
+    <t>tab_5_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">## How has the data for demand been calculated?
+The calls generated in the model are randomly generated, but broadly will follow the patterns seen historically in 2023 and 2024.
+This includes data on 
+- calls which were attended by a DAAT resource
+- calls which were identified as appropriate for HEMS intervention, but were not attended due to no appropriate DAAT resource being available at the time
+- calls received during the hours in which no HEMS resource was on shift, which were identified by the HEMS desk team as calls received in the period which would have had a resource sent had one been available
+## Isn't this an underestimate of the true demand?
+While we are using Devon Air Ambulance data rather than the raw data from the South West Ambulance Service Trust, by including the additional 'missed' calls we are more closely approximating the actual demand that is seen across the region. 
+Ambulance service data and other data sets may be reviewed in a later version of the model to assess whether there is additional demand that is not being met. However, at present it is also possible to manually adjust the demand in the model by a percentage, resulting in an increased number of calls being generated per day. In this way, you can explore the possible impact on resources if the pool of suitable HEMS cases is predicted to increase over time, or if it is anticipated that more HEMS-suitable cases could be identified.  
+## Why don't we just use exact historical call times in the model?
+Air ambulance services experience relatively low demand volumes compared to, for example, an ambulance trust or a service like 111. While there are observed patterns relating to the number of calls that come in across different times of year, day of the week and time of day, the calls are not influenced by one another. To best explore the full spectrum of possible call arrival patterns and best see how the service copes on a wide variety of plausible days, we take these historical patterns can calculate a mathematical representation of the call arrival patterns. We can then use this to generate an infinite stream of calls that allow us to test the system. 
+## Is any data excluded when calculating demand?
+At present, we do not include demand relating solely to patient transport. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## How are stand-downs calculated?
+The proportion of calls which are stood down prior to mobilisation and en route, and the proportion of calls which transfer the patient from the scene, also follow historical patterns. 
+This then goes on to affect the way in which the call unfolds - for example, a call which is stood down en route will have allocation time, mobilitation time, and time to clear. 
+## What factors affect stand-down rate in the model?
+When determining the chance of a given call being stood down, this is based on historical patterns observed for both the callsign group and the type of vehicle (car vs helicopter) being dispatched. Other possible outcomes beyond the call being stood down before mobilisation or en route are
+- landed, but no patient contact
+- treated (not conveyed)
+- conveyed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">## How are the durations of calls calculated?
+Two years of data have been looked at to generate mathematical representations of each step of the process of attending a call, split by whether a call is being attended by a car or a helicopter. 
+For each call generated within the model, we will generate the following times:
+- time to allocate
+- time to mobilise
+- time to travel to scene
+- time on scene
+- time travelling to hospital
+- time to clear
+Not every call will complete every stage of the process - for example, a call that is stood down en route will not spend time on scene or travelling to a hospital. 
+## Why are the times for each step of the process only affected by whether the resource is a car or a helicopter?
+The historical data on calls was thoroughly investigated to determine the aspects which should be incorporated when generating appropriate durations for different parts of the patient journey. 
+Clear differences were seen in average durations and variation in durations when splitting calls by vehicle type, without reducing the pool of calls being analysed to very small numbers. 
+Computer simulation often requires a balance of modelling the nuances of real-world systems with simplifying them down. While it would be possible to also bring in factors like the AMPDS card, subdividing our pool of historical calls more and more can lead to the model becoming overly complex, which can actually reduce its ability to helpfully represent our real-world system. </t>
+  </si>
+  <si>
+    <t>Resource Allocation</t>
+  </si>
+  <si>
+    <t>## How does the model decide which resource to allocate to a call? 
+Coming soon!</t>
   </si>
 </sst>
 </file>
@@ -516,7 +556,7 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +573,7 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -676,7 +716,7 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -684,7 +724,7 @@
         <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -805,26 +845,26 @@
     </row>
     <row r="2" spans="1:2" ht="76.5">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="39" customHeight="1">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -930,10 +970,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67EDA8F5-689A-46D5-BBAC-DC7FC0FF134A}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -958,12 +998,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="102">
+    <row r="3" spans="1:2" ht="114.75">
       <c r="A3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -971,7 +1011,7 @@
         <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -979,7 +1019,7 @@
         <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -987,47 +1027,63 @@
         <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="63.75">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="409.5">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="409.5">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="242.25">
+      <c r="A12" t="s">
         <v>65</v>
       </c>
-      <c r="B7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="63.75">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="89.25">
-      <c r="A9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="38.25">
-      <c r="A10" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="38.25">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>68</v>
+      <c r="B12" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="38.25">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>